<commit_message>
Creation d'un programme Wifi IO avec MQTT Diverses finalisations et tests: - Test 4 Oyas + pompe + master OK - Pompage wifi io tjs ok / boutlot avec Paul
</commit_message>
<xml_diff>
--- a/jarduino2/jard_485_slave/board/nomenclature.xlsx
+++ b/jarduino2/jard_485_slave/board/nomenclature.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEV\GITHUB\modules_uino\jarduino2\OyaSyst\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEV\GITHUB\modules_uino\jarduino2\jard_485_slave\board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D83AAB9-872D-4D09-A80F-8A340C67CE57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7FCE0E6-CA62-4F48-B22C-411DAD60CF38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Mods" sheetId="1" r:id="rId1"/>
-    <sheet name="CMS" sheetId="2" r:id="rId2"/>
-    <sheet name="THT" sheetId="3" r:id="rId3"/>
+    <sheet name="Ensemble" sheetId="4" r:id="rId1"/>
+    <sheet name="Carte Mods" sheetId="1" r:id="rId2"/>
+    <sheet name="CMS" sheetId="2" r:id="rId3"/>
+    <sheet name="THT" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="65">
   <si>
     <t>Nano 168P</t>
   </si>
@@ -121,9 +122,6 @@
     <t>Résistances 100k</t>
   </si>
   <si>
-    <t>Diode</t>
-  </si>
-  <si>
     <t>Résistance 150</t>
   </si>
   <si>
@@ -139,17 +137,110 @@
     <t>Capa 10nF</t>
   </si>
   <si>
-    <t>Transistor TIP41C NPN</t>
-  </si>
-  <si>
     <t>Farnel</t>
+  </si>
+  <si>
+    <t>Carte CI + composants</t>
+  </si>
+  <si>
+    <t>Capa 100nF</t>
+  </si>
+  <si>
+    <t>Bornier 3 contacts à vis</t>
+  </si>
+  <si>
+    <t>Diode de redressement</t>
+  </si>
+  <si>
+    <t>Diode de protection</t>
+  </si>
+  <si>
+    <t>Transistor P03P4L-04</t>
+  </si>
+  <si>
+    <t>Transistor 2N2222</t>
+  </si>
+  <si>
+    <t>Résistance 40k</t>
+  </si>
+  <si>
+    <t>Résistance 10k</t>
+  </si>
+  <si>
+    <t>Résistance 30mR</t>
+  </si>
+  <si>
+    <t>Résistance 1k</t>
+  </si>
+  <si>
+    <t>Résistance 32k</t>
+  </si>
+  <si>
+    <t>DHT22</t>
+  </si>
+  <si>
+    <t>AOP LM358</t>
+  </si>
+  <si>
+    <t>https://fr.aliexpress.com/item/1005002656127438.html?spm=a2g0o.productlist.main.115.6fec7157O1de8N&amp;algo_pvid=b84d91b7-697f-49dd-a2ac-2cf5aaf269d9&amp;algo_exp_id=b84d91b7-697f-49dd-a2ac-2cf5aaf269d9-57&amp;pdp_npi=3%40dis%21EUR%219.32%219.32%21%21%21%21%21%402100bb6416843492275713328d077e%2112000021579672741%21sea%21FR%212150986022&amp;curPageLogUid=4WkS0xZRCrQT</t>
+  </si>
+  <si>
+    <t>https://fr.aliexpress.com/item/1005004095263998.html?pdp_npi=2%40dis%21EUR%211%2C59%E2%82%AC%211%2C59%E2%82%AC%21%21%21%21%21%40211b80e116843497260067342ebb57%2112000028024520932%21btf&amp;_t=pvid%3A9c2b7dc5-9b42-4f98-ae02-fc9ca62ed9d3&amp;afTraceInfo=1005004095263998__pc__pcBridgePPC__xxxxxx__1684349726&amp;spm=a2g0o.ppclist.product.mainProduct&amp;gatewayAdapt=glo2fra</t>
+  </si>
+  <si>
+    <t>https://fr.aliexpress.com/item/1005003507912340.html?spm=a2g0o.productlist.main.7.3ac03edc17Wpm4&amp;algo_pvid=20f14c10-48fe-4db0-a823-2bbce76535ba&amp;aem_p4p_detail=20230517115719268119078755670004592397&amp;algo_exp_id=20f14c10-48fe-4db0-a823-2bbce76535ba-3&amp;pdp_npi=3%40dis%21EUR%210.91%210.82%21%21%21%21%21%402145274c16843498390178553d0744%2112000026103587637%21sea%21FR%212150986022&amp;curPageLogUid=ZY2jVpYmhSdq&amp;ad_pvid=20230517115719268119078755670004592397_4&amp;ad_pvid=20230517115719268119078755670004592397_4</t>
+  </si>
+  <si>
+    <t>Circuit imprimé</t>
+  </si>
+  <si>
+    <t>Fils</t>
+  </si>
+  <si>
+    <t>Cosses</t>
+  </si>
+  <si>
+    <t>Boîte de dérivation</t>
+  </si>
+  <si>
+    <t>Raccord T 12mm</t>
+  </si>
+  <si>
+    <t>Racord coude 12mm et 10mm</t>
+  </si>
+  <si>
+    <t>Colliers 10mm</t>
+  </si>
+  <si>
+    <t>Colliers 12mm</t>
+  </si>
+  <si>
+    <t>Dessous de vase</t>
+  </si>
+  <si>
+    <t>Ecrous</t>
+  </si>
+  <si>
+    <t>Boulons tête fraisée</t>
+  </si>
+  <si>
+    <t>Rondelles</t>
+  </si>
+  <si>
+    <t>Tuyau 10 mm (en m)</t>
+  </si>
+  <si>
+    <t>https://fr.aliexpress.com/item/1005001677869988.html?spm=a2g0o.order_detail.order_detail_item.3.450b7d568tyF3d&amp;gatewayAdapt=glo2fra</t>
+  </si>
+  <si>
+    <t>Casto</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,6 +260,19 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -195,7 +299,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -205,6 +309,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -485,20 +591,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D2:J27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{850E4AF3-F92A-479A-9410-CF674473282F}">
+  <dimension ref="D2:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="33.44140625" customWidth="1"/>
-    <col min="10" max="10" width="255.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.42578125" customWidth="1"/>
+    <col min="10" max="10" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
@@ -507,7 +613,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="4:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="4:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
@@ -521,261 +627,317 @@
         <v>7</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="E4">
-        <v>2.91</v>
+        <f>'Carte Mods'!G29</f>
+        <v>25.228999999999999</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4">
         <f>E4*F4</f>
-        <v>2.91</v>
-      </c>
-    </row>
-    <row r="5" spans="4:10" x14ac:dyDescent="0.3">
+        <v>25.228999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E5">
-        <v>0.7</v>
+        <v>5.41</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5">
-        <f t="shared" ref="G5:G17" si="0">E5*F5</f>
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="6" spans="4:10" x14ac:dyDescent="0.3">
+        <f t="shared" ref="G5:G22" si="0">E5*F5</f>
+        <v>5.41</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E6">
-        <v>1.61</v>
+        <v>4.88</v>
       </c>
       <c r="F6">
         <v>2</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>3.22</v>
-      </c>
-    </row>
-    <row r="7" spans="4:10" x14ac:dyDescent="0.3">
+        <v>9.76</v>
+      </c>
+      <c r="J6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="E7">
-        <v>1.06</v>
+        <f>1.94/2</f>
+        <v>0.97</v>
       </c>
       <c r="F7">
+        <v>0.2</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>0.19400000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8">
+        <f>1.76/50</f>
+        <v>3.5200000000000002E-2</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>7.0400000000000004E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9">
+        <v>2.5</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="10" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10">
+        <f>5.86/3</f>
+        <v>1.9533333333333334</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>1.9533333333333334</v>
+      </c>
+    </row>
+    <row r="11" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11">
+        <f>1.46/5</f>
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>0.29199999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12">
+        <f>10.9/5</f>
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="F12">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>0.30520000000000003</v>
+      </c>
+      <c r="J12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13">
+        <f>2.92/10</f>
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>0.58399999999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14">
+        <f>2.74/10</f>
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>0.27400000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15">
+        <v>2.85</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>2.85</v>
+      </c>
+    </row>
+    <row r="16" spans="4:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D16" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="F16" s="5">
+        <v>4</v>
+      </c>
+      <c r="G16" s="5">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="17" spans="4:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="F17" s="5">
+        <v>4</v>
+      </c>
+      <c r="G17" s="5">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="18" spans="4:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="5">
+        <v>0.04</v>
+      </c>
+      <c r="F18" s="5">
+        <v>4</v>
+      </c>
+      <c r="G18" s="5">
+        <f t="shared" si="0"/>
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="19" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="F23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="2">
+        <f>SUM(G4:G22)</f>
+        <v>51.181933333333333</v>
+      </c>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="27" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G7">
-        <f t="shared" si="0"/>
-        <v>3.18</v>
-      </c>
-    </row>
-    <row r="8" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8">
-        <v>5.41</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="0"/>
-        <v>5.41</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9">
-        <v>4.88</v>
-      </c>
-      <c r="F9">
-        <v>2</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="0"/>
-        <v>9.76</v>
-      </c>
-      <c r="J9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10">
-        <v>0.03</v>
-      </c>
-      <c r="F10">
-        <v>4</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="0"/>
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="11" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D11" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11">
-        <v>0.03</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="0"/>
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="12" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12">
-        <v>0.2</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="13" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D13" t="s">
-        <v>30</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D14" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D15" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15">
-        <v>2</v>
-      </c>
-      <c r="G15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D16" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16">
-        <v>0.5</v>
-      </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="17" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E17">
-        <v>0.72</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17">
-        <f t="shared" si="0"/>
-        <v>0.72</v>
-      </c>
-      <c r="H17">
-        <v>9804170</v>
-      </c>
-    </row>
-    <row r="21" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="F21" s="2" t="s">
+    </row>
+    <row r="28" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28">
         <v>12</v>
       </c>
-      <c r="G21" s="2">
-        <f>SUM(G4:G20)</f>
-        <v>26.75</v>
-      </c>
-      <c r="H21" s="2"/>
-    </row>
-    <row r="25" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D25" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D26" t="s">
-        <v>18</v>
-      </c>
-      <c r="E26">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D27" t="s">
+    </row>
+    <row r="29" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
         <v>1</v>
       </c>
     </row>
@@ -784,7 +946,7 @@
     <mergeCell ref="D2:G2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="J8" r:id="rId1" xr:uid="{78885027-6312-409A-A44A-FE170E149A31}"/>
+    <hyperlink ref="J5" r:id="rId1" xr:uid="{FDFE0B5B-2938-46E2-BB31-2FE201BD79A2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
@@ -792,28 +954,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83B0F0D9-2187-4C02-8EF8-2B3242F54C0F}">
-  <dimension ref="D2:I20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="D2:J35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="33.44140625" customWidth="1"/>
-    <col min="9" max="9" width="255.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.42578125" customWidth="1"/>
+    <col min="10" max="10" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="4:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="4:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
@@ -826,11 +989,14 @@
       <c r="G3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="H3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>0</v>
       </c>
@@ -845,7 +1011,7 @@
         <v>2.91</v>
       </c>
     </row>
-    <row r="5" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>1</v>
       </c>
@@ -856,11 +1022,483 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <f t="shared" ref="G5:G10" si="0">E5*F5</f>
+        <f t="shared" ref="G5:G27" si="0">E5*F5</f>
         <v>0.7</v>
       </c>
     </row>
-    <row r="6" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <f>(1.58+1.62)/5</f>
+        <v>0.64</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>1.28</v>
+      </c>
+    </row>
+    <row r="7" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <f>(1.05+1.62)/5</f>
+        <v>0.53400000000000003</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>0.53400000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="4:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="6">
+        <f>(1.32+1.62)/5</f>
+        <v>0.58800000000000008</v>
+      </c>
+      <c r="F8" s="6">
+        <v>2</v>
+      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9">
+        <v>0.03</v>
+      </c>
+      <c r="F9">
+        <v>7</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="10" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10">
+        <v>0.03</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="11" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11">
+        <v>0.2</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="12" spans="4:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="5">
+        <v>1</v>
+      </c>
+      <c r="F12" s="5">
+        <v>1</v>
+      </c>
+      <c r="G12" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="4:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="F13" s="5">
+        <v>1</v>
+      </c>
+      <c r="G13" s="5">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="4:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="F14" s="5">
+        <v>1</v>
+      </c>
+      <c r="G14" s="5">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="4:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="F15" s="5">
+        <v>2</v>
+      </c>
+      <c r="G15" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16">
+        <v>0.5</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="6">
+        <v>1.52</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>1.52</v>
+      </c>
+    </row>
+    <row r="18" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="F18">
+        <v>3</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="19" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19">
+        <f>(9.32+5.17)/10</f>
+        <v>1.4490000000000001</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>1.4490000000000001</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="4:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20">
+        <v>0.03</v>
+      </c>
+      <c r="F20" s="5">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="21" spans="4:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21">
+        <v>0.03</v>
+      </c>
+      <c r="F21" s="5">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="22" spans="4:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22">
+        <v>0.03</v>
+      </c>
+      <c r="F22" s="5">
+        <v>3</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="23" spans="4:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D23" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23">
+        <v>0.03</v>
+      </c>
+      <c r="F23" s="5">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="24" spans="4:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D24" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24">
+        <v>0.03</v>
+      </c>
+      <c r="F24" s="5">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="25" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25">
+        <v>1.59</v>
+      </c>
+      <c r="F25" s="5">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>1.59</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>46</v>
+      </c>
+      <c r="E26">
+        <f>(0.82+1.54)/10</f>
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="F26" s="5">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D27" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E27" s="6">
+        <v>9.33</v>
+      </c>
+      <c r="F27" s="6">
+        <v>1</v>
+      </c>
+      <c r="G27" s="6">
+        <f t="shared" si="0"/>
+        <v>9.33</v>
+      </c>
+    </row>
+    <row r="29" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="F29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29" s="2">
+        <f>SUM(G4:G28)</f>
+        <v>25.228999999999999</v>
+      </c>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="33" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D33" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>18</v>
+      </c>
+      <c r="E34">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D2:G2"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="J19" r:id="rId1" display="https://fr.aliexpress.com/item/1005002656127438.html?spm=a2g0o.productlist.main.115.6fec7157O1de8N&amp;algo_pvid=b84d91b7-697f-49dd-a2ac-2cf5aaf269d9&amp;algo_exp_id=b84d91b7-697f-49dd-a2ac-2cf5aaf269d9-57&amp;pdp_npi=3%40dis%21EUR%219.32%219.32%21%21%21%21%21%402100bb6416843492275713328d077e%2112000021579672741%21sea%21FR%212150986022&amp;curPageLogUid=4WkS0xZRCrQT" xr:uid="{DE400DFC-7EDB-4207-AF25-026F24ADBC89}"/>
+    <hyperlink ref="J25" r:id="rId2" display="https://fr.aliexpress.com/item/1005004095263998.html?pdp_npi=2%40dis%21EUR%211%2C59%E2%82%AC%211%2C59%E2%82%AC%21%21%21%21%21%40211b80e116843497260067342ebb57%2112000028024520932%21btf&amp;_t=pvid%3A9c2b7dc5-9b42-4f98-ae02-fc9ca62ed9d3&amp;afTraceInfo=1005004095263998__pc__pcBridgePPC__xxxxxx__1684349726&amp;spm=a2g0o.ppclist.product.mainProduct&amp;gatewayAdapt=glo2fra" xr:uid="{B9AFC7C6-1266-47FD-A2D1-8663805C64D3}"/>
+    <hyperlink ref="J26" r:id="rId3" display="https://fr.aliexpress.com/item/1005003507912340.html?spm=a2g0o.productlist.main.7.3ac03edc17Wpm4&amp;algo_pvid=20f14c10-48fe-4db0-a823-2bbce76535ba&amp;aem_p4p_detail=20230517115719268119078755670004592397&amp;algo_exp_id=20f14c10-48fe-4db0-a823-2bbce76535ba-3&amp;pdp_npi=3%40dis%21EUR%210.91%210.82%21%21%21%21%21%402145274c16843498390178553d0744%2112000026103587637%21sea%21FR%212150986022&amp;curPageLogUid=ZY2jVpYmhSdq&amp;ad_pvid=20230517115719268119078755670004592397_4&amp;ad_pvid=20230517115719268119078755670004592397_4" xr:uid="{E05E8D0F-B251-47ED-8FED-28DB62E98058}"/>
+    <hyperlink ref="J8" r:id="rId4" xr:uid="{407E9CCE-B363-4154-9F82-EFD8D41ACD3A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83B0F0D9-2187-4C02-8EF8-2B3242F54C0F}">
+  <dimension ref="D2:I18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="33.42578125" customWidth="1"/>
+    <col min="9" max="9" width="255.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="4:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>2.91</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <f>E4*F4</f>
+        <v>2.91</v>
+      </c>
+    </row>
+    <row r="5" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0.7</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ref="G5:G8" si="0">E5*F5</f>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="6" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>4</v>
       </c>
@@ -878,7 +1516,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>5</v>
       </c>
@@ -893,7 +1531,7 @@
         <v>3.22</v>
       </c>
     </row>
-    <row r="8" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>6</v>
       </c>
@@ -908,79 +1546,43 @@
         <v>2.12</v>
       </c>
     </row>
-    <row r="9" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9">
-        <v>5.41</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="0"/>
-        <v>5.41</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10">
-        <v>4.88</v>
-      </c>
-      <c r="F10">
-        <v>2</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="0"/>
-        <v>9.76</v>
-      </c>
-      <c r="I10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="F14" s="2" t="s">
+    <row r="12" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="F12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="2">
-        <f>SUM(G4:G13)</f>
-        <v>24.93</v>
-      </c>
-    </row>
-    <row r="18" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D18" s="2" t="s">
+      <c r="G12" s="2">
+        <f>SUM(G4:G11)</f>
+        <v>9.7600000000000016</v>
+      </c>
+    </row>
+    <row r="16" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G16" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2" t="s">
+      <c r="H16" s="2"/>
+      <c r="I16" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D19" t="s">
+    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
         <v>18</v>
       </c>
-      <c r="E19">
+      <c r="E17">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D20" t="s">
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
         <v>1</v>
       </c>
     </row>
@@ -990,28 +1592,27 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I6" r:id="rId1" display="https://fr.aliexpress.com/item/32835853612.html?spm=a2g0o.productlist.0.0.7fd75a460WZR74&amp;algo_pvid=04dc54b6-97ab-4205-9332-30ac5554ce0c&amp;aem_p4p_detail=20221126095913764170344110700001964064&amp;algo_exp_id=04dc54b6-97ab-4205-9332-30ac5554ce0c-0&amp;pdp_ext_f=%7B%22sku_id%22%3A%2212000025152727956%22%7D&amp;pdp_npi=2%40dis%21EUR%210.93%210.81%21%21%21%21%21%400b0a050b16694855532033144ec78b%2112000025152727956%21sea&amp;curPageLogUid=CfbSgzYXkdFU&amp;ad_pvid=20221126095913764170344110700001964064_1&amp;ad_pvid=20221126095913764170344110700001964064_1" xr:uid="{6E360586-6742-4D2D-89C9-0ABA883350D8}"/>
-    <hyperlink ref="I9" r:id="rId2" xr:uid="{4AE1F372-E556-4090-A0C9-BCDA353D7749}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A305140-1C6A-4CAB-954C-33C2E052E9C3}">
-  <dimension ref="D2:I25"/>
+  <dimension ref="D2:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="33.44140625" customWidth="1"/>
-    <col min="9" max="9" width="255.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.42578125" customWidth="1"/>
+    <col min="9" max="9" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
@@ -1019,7 +1620,7 @@
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="4:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="4:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
@@ -1036,7 +1637,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>19</v>
       </c>
@@ -1051,7 +1652,7 @@
         <v>4.28</v>
       </c>
     </row>
-    <row r="5" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>20</v>
       </c>
@@ -1066,7 +1667,7 @@
         <v>0.104</v>
       </c>
     </row>
-    <row r="6" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>21</v>
       </c>
@@ -1081,7 +1682,7 @@
         <v>3.9E-2</v>
       </c>
     </row>
-    <row r="7" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>22</v>
       </c>
@@ -1096,7 +1697,7 @@
         <v>0.214</v>
       </c>
     </row>
-    <row r="8" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>23</v>
       </c>
@@ -1111,7 +1712,7 @@
         <v>0.38700000000000001</v>
       </c>
     </row>
-    <row r="9" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>24</v>
       </c>
@@ -1122,11 +1723,11 @@
         <v>6.04</v>
       </c>
       <c r="G9">
-        <f t="shared" ref="G9:G15" si="1">E9*F9</f>
+        <f t="shared" ref="G9:G13" si="1">E9*F9</f>
         <v>6.04</v>
       </c>
     </row>
-    <row r="10" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>25</v>
       </c>
@@ -1141,7 +1742,7 @@
         <v>0.72199999999999998</v>
       </c>
     </row>
-    <row r="11" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>4</v>
       </c>
@@ -1159,7 +1760,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>5</v>
       </c>
@@ -1174,7 +1775,7 @@
         <v>3.22</v>
       </c>
     </row>
-    <row r="13" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>6</v>
       </c>
@@ -1189,79 +1790,43 @@
         <v>2.12</v>
       </c>
     </row>
-    <row r="14" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14">
-        <v>5.41</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14">
-        <f t="shared" si="1"/>
-        <v>5.41</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15">
-        <v>4.88</v>
-      </c>
-      <c r="F15">
-        <v>2</v>
-      </c>
-      <c r="G15">
-        <f t="shared" si="1"/>
-        <v>9.76</v>
-      </c>
-      <c r="I15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="F19" s="2" t="s">
+    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="F17" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="2">
-        <f>SUM(G4:G18)</f>
-        <v>33.106000000000002</v>
-      </c>
-    </row>
-    <row r="23" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D23" s="2" t="s">
+      <c r="G17" s="2">
+        <f>SUM(G4:G16)</f>
+        <v>17.936</v>
+      </c>
+    </row>
+    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G21" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2" t="s">
+      <c r="H21" s="2"/>
+      <c r="I21" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D24" t="s">
+    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
         <v>18</v>
       </c>
-      <c r="E24">
+      <c r="E22">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D25" t="s">
+    <row r="23" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1271,9 +1836,8 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I11" r:id="rId1" display="https://fr.aliexpress.com/item/32835853612.html?spm=a2g0o.productlist.0.0.7fd75a460WZR74&amp;algo_pvid=04dc54b6-97ab-4205-9332-30ac5554ce0c&amp;aem_p4p_detail=20221126095913764170344110700001964064&amp;algo_exp_id=04dc54b6-97ab-4205-9332-30ac5554ce0c-0&amp;pdp_ext_f=%7B%22sku_id%22%3A%2212000025152727956%22%7D&amp;pdp_npi=2%40dis%21EUR%210.93%210.81%21%21%21%21%21%400b0a050b16694855532033144ec78b%2112000025152727956%21sea&amp;curPageLogUid=CfbSgzYXkdFU&amp;ad_pvid=20221126095913764170344110700001964064_1&amp;ad_pvid=20221126095913764170344110700001964064_1" xr:uid="{76F40083-0976-42D4-B60F-B4C747AD57E2}"/>
-    <hyperlink ref="I14" r:id="rId2" xr:uid="{EAAD93AD-39CE-4B65-AAB3-EF8DF6EF5186}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>